<commit_message>
Work on data tyding
</commit_message>
<xml_diff>
--- a/data/table_electricity_case_study.xlsx
+++ b/data/table_electricity_case_study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudolfs Lukasevics\OneDrive - College of the Atlantic\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8DEE2F-A5FA-4782-BE17-76C1B816DD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE33FB27-6A58-47CA-A84E-6D4C7D8AAE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12652" xr2:uid="{9BFCAE98-E176-4C8F-8980-DE4A0FFE9217}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="21">
   <si>
     <t>Month</t>
   </si>
@@ -62,43 +62,43 @@
     <t>Building</t>
   </si>
   <si>
-    <t>July</t>
+    <t>Year</t>
   </si>
   <si>
-    <t>August</t>
+    <t>07</t>
   </si>
   <si>
-    <t>September</t>
+    <t>08</t>
   </si>
   <si>
-    <t>October</t>
+    <t>09</t>
   </si>
   <si>
-    <t>November</t>
+    <t>01</t>
   </si>
   <si>
-    <t>December</t>
+    <t>02</t>
   </si>
   <si>
-    <t>January</t>
+    <t>03</t>
   </si>
   <si>
-    <t>February</t>
+    <t>04</t>
   </si>
   <si>
-    <t>March</t>
+    <t>05</t>
   </si>
   <si>
-    <t>April</t>
+    <t>06</t>
   </si>
   <si>
-    <t>May</t>
+    <t>12</t>
   </si>
   <si>
-    <t>June</t>
+    <t>10</t>
   </si>
   <si>
-    <t>Year</t>
+    <t>11</t>
   </si>
 </sst>
 </file>
@@ -146,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -155,6 +155,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7EC2C1A-A8D4-4442-9E0B-12AB32A32C92}">
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -505,7 +506,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -518,8 +519,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>8</v>
+      <c r="A2" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B2">
         <v>2019</v>
@@ -535,8 +536,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>9</v>
+      <c r="A3" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B3">
         <v>2019</v>
@@ -552,8 +553,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>10</v>
+      <c r="A4" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B4">
         <v>2019</v>
@@ -569,8 +570,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>11</v>
+      <c r="A5" s="4">
+        <v>10</v>
       </c>
       <c r="B5">
         <v>2019</v>
@@ -586,8 +587,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>12</v>
+      <c r="A6" s="4">
+        <v>11</v>
       </c>
       <c r="B6">
         <v>2019</v>
@@ -603,8 +604,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>13</v>
+      <c r="A7" s="4">
+        <v>12</v>
       </c>
       <c r="B7">
         <v>2019</v>
@@ -620,8 +621,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>14</v>
+      <c r="A8" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B8">
         <v>2020</v>
@@ -637,8 +638,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>15</v>
+      <c r="A9" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B9">
         <v>2020</v>
@@ -654,8 +655,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>16</v>
+      <c r="A10" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B10">
         <v>2020</v>
@@ -671,8 +672,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>17</v>
+      <c r="A11" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B11">
         <v>2020</v>
@@ -688,8 +689,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>18</v>
+      <c r="A12" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B12">
         <v>2020</v>
@@ -705,8 +706,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>19</v>
+      <c r="A13" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B13">
         <v>2020</v>
@@ -722,8 +723,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>8</v>
+      <c r="A14" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B14">
         <v>2020</v>
@@ -739,8 +740,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>9</v>
+      <c r="A15" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B15">
         <v>2020</v>
@@ -756,8 +757,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>10</v>
+      <c r="A16" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B16">
         <v>2020</v>
@@ -773,8 +774,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>11</v>
+      <c r="A17" s="4">
+        <v>10</v>
       </c>
       <c r="B17">
         <v>2020</v>
@@ -790,8 +791,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>12</v>
+      <c r="A18" s="4">
+        <v>11</v>
       </c>
       <c r="B18">
         <v>2020</v>
@@ -807,8 +808,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>13</v>
+      <c r="A19" s="4">
+        <v>12</v>
       </c>
       <c r="B19">
         <v>2020</v>
@@ -824,8 +825,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>14</v>
+      <c r="A20" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B20">
         <v>2021</v>
@@ -841,8 +842,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>15</v>
+      <c r="A21" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B21">
         <v>2021</v>
@@ -858,8 +859,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>16</v>
+      <c r="A22" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B22">
         <v>2021</v>
@@ -875,8 +876,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>17</v>
+      <c r="A23" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B23">
         <v>2021</v>
@@ -892,8 +893,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>18</v>
+      <c r="A24" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B24">
         <v>2021</v>
@@ -909,8 +910,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>19</v>
+      <c r="A25" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B25">
         <v>2021</v>
@@ -926,8 +927,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>8</v>
+      <c r="A26" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B26">
         <v>2021</v>
@@ -943,8 +944,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>9</v>
+      <c r="A27" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B27">
         <v>2021</v>
@@ -960,8 +961,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
-        <v>10</v>
+      <c r="A28" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B28">
         <v>2021</v>
@@ -977,8 +978,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>11</v>
+      <c r="A29" s="4">
+        <v>10</v>
       </c>
       <c r="B29">
         <v>2021</v>
@@ -994,8 +995,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>12</v>
+      <c r="A30" s="4">
+        <v>11</v>
       </c>
       <c r="B30">
         <v>2021</v>
@@ -1011,8 +1012,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
-        <v>13</v>
+      <c r="A31" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B31">
         <v>2021</v>
@@ -1028,8 +1029,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>14</v>
+      <c r="A32" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B32">
         <v>2022</v>
@@ -1045,8 +1046,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
-        <v>15</v>
+      <c r="A33" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B33">
         <v>2022</v>
@@ -1062,8 +1063,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
-        <v>16</v>
+      <c r="A34" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B34">
         <v>2022</v>
@@ -1079,8 +1080,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>17</v>
+      <c r="A35" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B35">
         <v>2022</v>
@@ -1096,8 +1097,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>18</v>
+      <c r="A36" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B36">
         <v>2022</v>
@@ -1113,8 +1114,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
-        <v>19</v>
+      <c r="A37" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B37">
         <v>2022</v>
@@ -1130,8 +1131,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
-        <v>8</v>
+      <c r="A38" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B38">
         <v>2022</v>
@@ -1147,8 +1148,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
-        <v>9</v>
+      <c r="A39" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B39">
         <v>2022</v>
@@ -1164,8 +1165,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>10</v>
+      <c r="A40" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B40">
         <v>2022</v>
@@ -1181,8 +1182,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
-        <v>11</v>
+      <c r="A41" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B41">
         <v>2022</v>
@@ -1198,8 +1199,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
-        <v>12</v>
+      <c r="A42" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="B42">
         <v>2022</v>
@@ -1215,8 +1216,8 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
-        <v>13</v>
+      <c r="A43" s="4">
+        <v>12</v>
       </c>
       <c r="B43">
         <v>2022</v>
@@ -1232,8 +1233,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
-        <v>14</v>
+      <c r="A44" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B44">
         <v>2023</v>
@@ -1249,8 +1250,8 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
-        <v>15</v>
+      <c r="A45" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B45">
         <v>2023</v>
@@ -1266,8 +1267,8 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
-        <v>16</v>
+      <c r="A46" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B46">
         <v>2023</v>
@@ -1283,8 +1284,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>17</v>
+      <c r="A47" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B47">
         <v>2023</v>
@@ -1300,8 +1301,8 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
-        <v>11</v>
+      <c r="A48" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B48">
         <v>2019</v>
@@ -1317,8 +1318,8 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A49" t="s">
-        <v>12</v>
+      <c r="A49" s="4">
+        <v>11</v>
       </c>
       <c r="B49">
         <v>2019</v>
@@ -1334,8 +1335,8 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
-        <v>13</v>
+      <c r="A50" s="4">
+        <v>12</v>
       </c>
       <c r="B50">
         <v>2019</v>
@@ -1351,8 +1352,8 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
-        <v>14</v>
+      <c r="A51" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B51">
         <v>2020</v>
@@ -1368,8 +1369,8 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
-        <v>15</v>
+      <c r="A52" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B52">
         <v>2020</v>
@@ -1385,8 +1386,8 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
-        <v>16</v>
+      <c r="A53" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B53">
         <v>2020</v>
@@ -1402,8 +1403,8 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A54" t="s">
-        <v>17</v>
+      <c r="A54" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B54">
         <v>2020</v>
@@ -1419,8 +1420,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
-        <v>18</v>
+      <c r="A55" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B55">
         <v>2020</v>
@@ -1436,8 +1437,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
-        <v>19</v>
+      <c r="A56" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B56">
         <v>2020</v>
@@ -1453,8 +1454,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
-        <v>8</v>
+      <c r="A57" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B57">
         <v>2020</v>
@@ -1470,8 +1471,8 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
-        <v>9</v>
+      <c r="A58" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B58">
         <v>2020</v>
@@ -1487,8 +1488,8 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
-        <v>10</v>
+      <c r="A59" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B59">
         <v>2020</v>
@@ -1504,8 +1505,8 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A60" t="s">
-        <v>11</v>
+      <c r="A60" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B60">
         <v>2020</v>
@@ -1521,8 +1522,8 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A61" t="s">
-        <v>12</v>
+      <c r="A61" s="4">
+        <v>11</v>
       </c>
       <c r="B61">
         <v>2020</v>
@@ -1538,8 +1539,8 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
-        <v>13</v>
+      <c r="A62" s="4">
+        <v>12</v>
       </c>
       <c r="B62">
         <v>2020</v>
@@ -1555,8 +1556,8 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A63" t="s">
-        <v>14</v>
+      <c r="A63" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B63">
         <v>2021</v>
@@ -1572,8 +1573,8 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A64" t="s">
-        <v>15</v>
+      <c r="A64" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B64">
         <v>2021</v>
@@ -1589,8 +1590,8 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A65" t="s">
-        <v>16</v>
+      <c r="A65" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B65">
         <v>2021</v>
@@ -1606,8 +1607,8 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A66" t="s">
-        <v>17</v>
+      <c r="A66" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B66">
         <v>2021</v>
@@ -1623,8 +1624,8 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A67" t="s">
-        <v>18</v>
+      <c r="A67" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B67">
         <v>2021</v>
@@ -1640,8 +1641,8 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A68" t="s">
-        <v>19</v>
+      <c r="A68" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B68">
         <v>2021</v>
@@ -1657,8 +1658,8 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A69" t="s">
-        <v>8</v>
+      <c r="A69" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B69">
         <v>2021</v>
@@ -1674,8 +1675,8 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A70" t="s">
-        <v>9</v>
+      <c r="A70" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B70">
         <v>2021</v>
@@ -1691,8 +1692,8 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A71" t="s">
-        <v>10</v>
+      <c r="A71" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B71">
         <v>2021</v>
@@ -1708,8 +1709,8 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A72" t="s">
-        <v>11</v>
+      <c r="A72" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B72">
         <v>2021</v>
@@ -1725,8 +1726,8 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A73" t="s">
-        <v>12</v>
+      <c r="A73" s="4">
+        <v>11</v>
       </c>
       <c r="B73">
         <v>2021</v>
@@ -1742,8 +1743,8 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A74" t="s">
-        <v>13</v>
+      <c r="A74" s="4">
+        <v>12</v>
       </c>
       <c r="B74">
         <v>2021</v>
@@ -1759,8 +1760,8 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A75" t="s">
-        <v>14</v>
+      <c r="A75" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B75">
         <v>2022</v>
@@ -1776,8 +1777,8 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A76" t="s">
-        <v>15</v>
+      <c r="A76" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B76">
         <v>2022</v>
@@ -1793,8 +1794,8 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A77" t="s">
-        <v>16</v>
+      <c r="A77" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B77">
         <v>2022</v>
@@ -1810,8 +1811,8 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A78" t="s">
-        <v>17</v>
+      <c r="A78" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B78">
         <v>2022</v>
@@ -1827,8 +1828,8 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A79" t="s">
-        <v>18</v>
+      <c r="A79" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B79">
         <v>2022</v>
@@ -1844,8 +1845,8 @@
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A80" t="s">
-        <v>19</v>
+      <c r="A80" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B80">
         <v>2022</v>
@@ -1861,8 +1862,8 @@
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A81" t="s">
-        <v>8</v>
+      <c r="A81" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B81">
         <v>2022</v>
@@ -1878,8 +1879,8 @@
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A82" t="s">
-        <v>9</v>
+      <c r="A82" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B82">
         <v>2022</v>
@@ -1895,8 +1896,8 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A83" t="s">
-        <v>8</v>
+      <c r="A83" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B83">
         <v>2019</v>
@@ -1912,8 +1913,8 @@
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A84" t="s">
-        <v>9</v>
+      <c r="A84" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B84">
         <v>2019</v>
@@ -1929,8 +1930,8 @@
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A85" t="s">
-        <v>10</v>
+      <c r="A85" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B85">
         <v>2019</v>
@@ -1946,8 +1947,8 @@
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A86" t="s">
-        <v>11</v>
+      <c r="A86" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B86">
         <v>2019</v>
@@ -1963,8 +1964,8 @@
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A87" t="s">
-        <v>12</v>
+      <c r="A87" s="4">
+        <v>11</v>
       </c>
       <c r="B87">
         <v>2019</v>
@@ -1980,8 +1981,8 @@
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A88" t="s">
-        <v>13</v>
+      <c r="A88" s="4">
+        <v>12</v>
       </c>
       <c r="B88">
         <v>2019</v>
@@ -1997,8 +1998,8 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A89" t="s">
-        <v>14</v>
+      <c r="A89" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B89">
         <v>2020</v>
@@ -2014,8 +2015,8 @@
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A90" t="s">
-        <v>15</v>
+      <c r="A90" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B90">
         <v>2020</v>
@@ -2031,8 +2032,8 @@
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A91" t="s">
-        <v>16</v>
+      <c r="A91" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B91">
         <v>2020</v>
@@ -2048,8 +2049,8 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A92" t="s">
-        <v>17</v>
+      <c r="A92" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B92">
         <v>2020</v>
@@ -2065,8 +2066,8 @@
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A93" t="s">
-        <v>18</v>
+      <c r="A93" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B93">
         <v>2020</v>
@@ -2082,8 +2083,8 @@
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A94" t="s">
-        <v>19</v>
+      <c r="A94" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B94">
         <v>2020</v>
@@ -2099,8 +2100,8 @@
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A95" t="s">
-        <v>8</v>
+      <c r="A95" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B95">
         <v>2020</v>
@@ -2116,8 +2117,8 @@
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A96" t="s">
-        <v>9</v>
+      <c r="A96" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B96">
         <v>2020</v>
@@ -2133,8 +2134,8 @@
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A97" t="s">
-        <v>10</v>
+      <c r="A97" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B97">
         <v>2020</v>
@@ -2150,8 +2151,8 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A98" t="s">
-        <v>11</v>
+      <c r="A98" s="4">
+        <v>10</v>
       </c>
       <c r="B98">
         <v>2020</v>
@@ -2167,8 +2168,8 @@
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A99" t="s">
-        <v>12</v>
+      <c r="A99" s="4">
+        <v>11</v>
       </c>
       <c r="B99">
         <v>2020</v>
@@ -2184,8 +2185,8 @@
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A100" t="s">
-        <v>13</v>
+      <c r="A100" s="4">
+        <v>12</v>
       </c>
       <c r="B100">
         <v>2020</v>
@@ -2201,8 +2202,8 @@
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A101" t="s">
-        <v>14</v>
+      <c r="A101" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B101">
         <v>2021</v>
@@ -2218,8 +2219,8 @@
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A102" t="s">
-        <v>15</v>
+      <c r="A102" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B102">
         <v>2021</v>
@@ -2235,8 +2236,8 @@
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A103" t="s">
-        <v>16</v>
+      <c r="A103" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B103">
         <v>2021</v>
@@ -2252,8 +2253,8 @@
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A104" t="s">
-        <v>17</v>
+      <c r="A104" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B104">
         <v>2021</v>
@@ -2269,8 +2270,8 @@
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A105" t="s">
-        <v>18</v>
+      <c r="A105" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B105">
         <v>2021</v>
@@ -2286,8 +2287,8 @@
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A106" t="s">
-        <v>19</v>
+      <c r="A106" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B106">
         <v>2021</v>
@@ -2303,8 +2304,8 @@
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A107" t="s">
-        <v>8</v>
+      <c r="A107" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B107">
         <v>2021</v>
@@ -2320,8 +2321,8 @@
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A108" t="s">
-        <v>9</v>
+      <c r="A108" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B108">
         <v>2021</v>
@@ -2337,8 +2338,8 @@
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A109" t="s">
-        <v>10</v>
+      <c r="A109" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B109">
         <v>2021</v>
@@ -2354,8 +2355,8 @@
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A110" t="s">
-        <v>11</v>
+      <c r="A110" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B110">
         <v>2021</v>
@@ -2371,8 +2372,8 @@
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A111" t="s">
-        <v>12</v>
+      <c r="A111" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="B111">
         <v>2021</v>
@@ -2388,8 +2389,8 @@
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A112" t="s">
-        <v>13</v>
+      <c r="A112" s="4">
+        <v>12</v>
       </c>
       <c r="B112">
         <v>2021</v>
@@ -2405,8 +2406,8 @@
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A113" t="s">
-        <v>14</v>
+      <c r="A113" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B113">
         <v>2022</v>
@@ -2422,8 +2423,8 @@
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A114" t="s">
-        <v>15</v>
+      <c r="A114" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B114">
         <v>2022</v>
@@ -2439,8 +2440,8 @@
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A115" t="s">
-        <v>16</v>
+      <c r="A115" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B115">
         <v>2022</v>
@@ -2456,8 +2457,8 @@
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A116" t="s">
-        <v>17</v>
+      <c r="A116" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B116">
         <v>2022</v>
@@ -2473,8 +2474,8 @@
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A117" t="s">
-        <v>18</v>
+      <c r="A117" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B117">
         <v>2022</v>
@@ -2490,8 +2491,8 @@
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A118" t="s">
-        <v>19</v>
+      <c r="A118" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B118">
         <v>2022</v>
@@ -2507,8 +2508,8 @@
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A119" t="s">
-        <v>8</v>
+      <c r="A119" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B119">
         <v>2022</v>
@@ -2524,8 +2525,8 @@
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A120" t="s">
-        <v>9</v>
+      <c r="A120" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B120">
         <v>2022</v>
@@ -2541,8 +2542,8 @@
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A121" t="s">
-        <v>12</v>
+      <c r="A121" s="4">
+        <v>11</v>
       </c>
       <c r="B121">
         <v>2019</v>
@@ -2558,8 +2559,8 @@
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A122" t="s">
-        <v>13</v>
+      <c r="A122" s="4">
+        <v>12</v>
       </c>
       <c r="B122">
         <v>2019</v>
@@ -2575,8 +2576,8 @@
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A123" t="s">
-        <v>14</v>
+      <c r="A123" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B123">
         <v>2020</v>
@@ -2592,8 +2593,8 @@
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A124" t="s">
-        <v>15</v>
+      <c r="A124" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B124">
         <v>2020</v>
@@ -2609,8 +2610,8 @@
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A125" t="s">
-        <v>16</v>
+      <c r="A125" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B125">
         <v>2020</v>
@@ -2626,8 +2627,8 @@
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A126" t="s">
-        <v>17</v>
+      <c r="A126" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B126">
         <v>2020</v>
@@ -2643,8 +2644,8 @@
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A127" t="s">
-        <v>18</v>
+      <c r="A127" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B127">
         <v>2020</v>
@@ -2660,8 +2661,8 @@
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A128" t="s">
-        <v>19</v>
+      <c r="A128" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B128">
         <v>2020</v>
@@ -2677,8 +2678,8 @@
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A129" t="s">
-        <v>8</v>
+      <c r="A129" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B129">
         <v>2020</v>
@@ -2694,8 +2695,8 @@
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A130" t="s">
-        <v>9</v>
+      <c r="A130" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B130">
         <v>2020</v>
@@ -2711,8 +2712,8 @@
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A131" t="s">
-        <v>10</v>
+      <c r="A131" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B131">
         <v>2020</v>
@@ -2728,8 +2729,8 @@
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A132" t="s">
-        <v>11</v>
+      <c r="A132" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B132">
         <v>2020</v>
@@ -2745,8 +2746,8 @@
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A133" t="s">
-        <v>12</v>
+      <c r="A133" s="4">
+        <v>11</v>
       </c>
       <c r="B133">
         <v>2020</v>
@@ -2762,8 +2763,8 @@
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A134" t="s">
-        <v>13</v>
+      <c r="A134" s="4">
+        <v>12</v>
       </c>
       <c r="B134">
         <v>2020</v>
@@ -2779,8 +2780,8 @@
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A135" t="s">
-        <v>14</v>
+      <c r="A135" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B135">
         <v>2021</v>
@@ -2796,8 +2797,8 @@
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A136" t="s">
-        <v>15</v>
+      <c r="A136" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B136">
         <v>2021</v>
@@ -2813,8 +2814,8 @@
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A137" t="s">
-        <v>16</v>
+      <c r="A137" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B137">
         <v>2021</v>
@@ -2830,8 +2831,8 @@
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A138" t="s">
-        <v>17</v>
+      <c r="A138" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B138">
         <v>2021</v>
@@ -2847,8 +2848,8 @@
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A139" t="s">
-        <v>18</v>
+      <c r="A139" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B139">
         <v>2021</v>
@@ -2864,8 +2865,8 @@
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A140" t="s">
-        <v>19</v>
+      <c r="A140" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B140">
         <v>2021</v>
@@ -2881,8 +2882,8 @@
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A141" t="s">
-        <v>8</v>
+      <c r="A141" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B141">
         <v>2021</v>
@@ -2898,8 +2899,8 @@
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A142" t="s">
-        <v>9</v>
+      <c r="A142" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B142">
         <v>2021</v>
@@ -2915,8 +2916,8 @@
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A143" t="s">
-        <v>10</v>
+      <c r="A143" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B143">
         <v>2021</v>
@@ -2932,8 +2933,8 @@
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A144" t="s">
-        <v>11</v>
+      <c r="A144" s="4">
+        <v>10</v>
       </c>
       <c r="B144">
         <v>2021</v>
@@ -2949,8 +2950,8 @@
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A145" t="s">
-        <v>12</v>
+      <c r="A145" s="4">
+        <v>11</v>
       </c>
       <c r="B145">
         <v>2021</v>
@@ -2966,8 +2967,8 @@
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A146" t="s">
-        <v>13</v>
+      <c r="A146" s="4">
+        <v>12</v>
       </c>
       <c r="B146">
         <v>2021</v>
@@ -2983,8 +2984,8 @@
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A147" t="s">
-        <v>14</v>
+      <c r="A147" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B147">
         <v>2022</v>
@@ -3000,8 +3001,8 @@
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A148" t="s">
-        <v>15</v>
+      <c r="A148" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B148">
         <v>2022</v>
@@ -3017,8 +3018,8 @@
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A149" t="s">
-        <v>16</v>
+      <c r="A149" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B149">
         <v>2022</v>
@@ -3034,8 +3035,8 @@
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A150" t="s">
-        <v>17</v>
+      <c r="A150" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B150">
         <v>2022</v>
@@ -3051,8 +3052,8 @@
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A151" t="s">
-        <v>18</v>
+      <c r="A151" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B151">
         <v>2022</v>
@@ -3068,8 +3069,8 @@
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A152" t="s">
-        <v>19</v>
+      <c r="A152" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B152">
         <v>2022</v>
@@ -3085,8 +3086,8 @@
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A153" t="s">
-        <v>8</v>
+      <c r="A153" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B153">
         <v>2022</v>
@@ -3104,5 +3105,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="150" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>